<commit_message>
adicionando resultados do SVM
</commit_message>
<xml_diff>
--- a/SVM/BOW/5folds/3/predict.xlsx
+++ b/SVM/BOW/5folds/3/predict.xlsx
@@ -7165,7 +7165,7 @@
         <v>0</v>
       </c>
       <c r="D229">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -8985,7 +8985,7 @@
         <v>0</v>
       </c>
       <c r="D359">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -9083,7 +9083,7 @@
         <v>0</v>
       </c>
       <c r="D366">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -9097,7 +9097,7 @@
         <v>0</v>
       </c>
       <c r="D367">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -9489,7 +9489,7 @@
         <v>0</v>
       </c>
       <c r="D395">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -9769,7 +9769,7 @@
         <v>1</v>
       </c>
       <c r="D415">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -10021,7 +10021,7 @@
         <v>0</v>
       </c>
       <c r="D433">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -10147,7 +10147,7 @@
         <v>0</v>
       </c>
       <c r="D442">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -10665,7 +10665,7 @@
         <v>0</v>
       </c>
       <c r="D479">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -10791,7 +10791,7 @@
         <v>0</v>
       </c>
       <c r="D488">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -10805,7 +10805,7 @@
         <v>0</v>
       </c>
       <c r="D489">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -10819,7 +10819,7 @@
         <v>1</v>
       </c>
       <c r="D490">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -11155,7 +11155,7 @@
         <v>0</v>
       </c>
       <c r="D514">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515" spans="1:4">
@@ -11715,7 +11715,7 @@
         <v>1</v>
       </c>
       <c r="D554">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="555" spans="1:4">
@@ -11883,7 +11883,7 @@
         <v>0</v>
       </c>
       <c r="D566">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="567" spans="1:4">
@@ -12177,7 +12177,7 @@
         <v>1</v>
       </c>
       <c r="D587">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="588" spans="1:4">
@@ -12821,7 +12821,7 @@
         <v>1</v>
       </c>
       <c r="D633">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -12863,7 +12863,7 @@
         <v>1</v>
       </c>
       <c r="D636">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="637" spans="1:4">
@@ -12877,7 +12877,7 @@
         <v>1</v>
       </c>
       <c r="D637">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="638" spans="1:4">
@@ -12947,7 +12947,7 @@
         <v>0</v>
       </c>
       <c r="D642">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="643" spans="1:4">
@@ -13717,7 +13717,7 @@
         <v>0</v>
       </c>
       <c r="D697">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="698" spans="1:4">
@@ -13759,7 +13759,7 @@
         <v>0</v>
       </c>
       <c r="D700">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="701" spans="1:4">
@@ -14179,7 +14179,7 @@
         <v>1</v>
       </c>
       <c r="D730">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="731" spans="1:4">
@@ -14221,7 +14221,7 @@
         <v>0</v>
       </c>
       <c r="D733">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="734" spans="1:4">
@@ -14963,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="D786">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="787" spans="1:4">
@@ -15733,7 +15733,7 @@
         <v>1</v>
       </c>
       <c r="D841">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="842" spans="1:4">
@@ -15957,7 +15957,7 @@
         <v>1</v>
       </c>
       <c r="D857">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="858" spans="1:4">
@@ -16069,7 +16069,7 @@
         <v>0</v>
       </c>
       <c r="D865">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="866" spans="1:4">
@@ -16111,7 +16111,7 @@
         <v>0</v>
       </c>
       <c r="D868">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="869" spans="1:4">
@@ -16167,7 +16167,7 @@
         <v>1</v>
       </c>
       <c r="D872">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="873" spans="1:4">
@@ -16321,7 +16321,7 @@
         <v>0</v>
       </c>
       <c r="D883">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="884" spans="1:4">
@@ -16671,7 +16671,7 @@
         <v>0</v>
       </c>
       <c r="D908">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="909" spans="1:4">
@@ -16825,7 +16825,7 @@
         <v>0</v>
       </c>
       <c r="D919">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="920" spans="1:4">
@@ -16895,7 +16895,7 @@
         <v>0</v>
       </c>
       <c r="D924">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="925" spans="1:4">
@@ -17567,7 +17567,7 @@
         <v>0</v>
       </c>
       <c r="D972">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="973" spans="1:4">
@@ -17595,7 +17595,7 @@
         <v>0</v>
       </c>
       <c r="D974">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="975" spans="1:4">
@@ -17735,7 +17735,7 @@
         <v>0</v>
       </c>
       <c r="D984">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="985" spans="1:4">
@@ -17819,7 +17819,7 @@
         <v>0</v>
       </c>
       <c r="D990">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="991" spans="1:4">
@@ -18169,7 +18169,7 @@
         <v>0</v>
       </c>
       <c r="D1015">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1016" spans="1:4">
@@ -18449,7 +18449,7 @@
         <v>0</v>
       </c>
       <c r="D1035">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1036" spans="1:4">
@@ -18659,7 +18659,7 @@
         <v>0</v>
       </c>
       <c r="D1050">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1051" spans="1:4">
@@ -18673,7 +18673,7 @@
         <v>0</v>
       </c>
       <c r="D1051">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1052" spans="1:4">
@@ -18729,7 +18729,7 @@
         <v>0</v>
       </c>
       <c r="D1055">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1056" spans="1:4">
@@ -18771,7 +18771,7 @@
         <v>0</v>
       </c>
       <c r="D1058">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1059" spans="1:4">
@@ -18911,7 +18911,7 @@
         <v>1</v>
       </c>
       <c r="D1068">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1069" spans="1:4">
@@ -19317,7 +19317,7 @@
         <v>0</v>
       </c>
       <c r="D1097">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1098" spans="1:4">
@@ -19443,7 +19443,7 @@
         <v>0</v>
       </c>
       <c r="D1106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1107" spans="1:4">
@@ -19485,7 +19485,7 @@
         <v>1</v>
       </c>
       <c r="D1109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1110" spans="1:4">
@@ -19681,7 +19681,7 @@
         <v>0</v>
       </c>
       <c r="D1123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1124" spans="1:4">
@@ -20661,7 +20661,7 @@
         <v>1</v>
       </c>
       <c r="D1193">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1194" spans="1:4">
@@ -20829,7 +20829,7 @@
         <v>0</v>
       </c>
       <c r="D1205">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1206" spans="1:4">
@@ -20871,7 +20871,7 @@
         <v>0</v>
       </c>
       <c r="D1208">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1209" spans="1:4">
@@ -21053,7 +21053,7 @@
         <v>0</v>
       </c>
       <c r="D1221">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1222" spans="1:4">
@@ -21151,7 +21151,7 @@
         <v>0</v>
       </c>
       <c r="D1228">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1229" spans="1:4">
@@ -21291,7 +21291,7 @@
         <v>1</v>
       </c>
       <c r="D1238">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1239" spans="1:4">
@@ -21487,7 +21487,7 @@
         <v>0</v>
       </c>
       <c r="D1252">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1253" spans="1:4">
@@ -21683,7 +21683,7 @@
         <v>1</v>
       </c>
       <c r="D1266">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1267" spans="1:4">
@@ -21851,7 +21851,7 @@
         <v>1</v>
       </c>
       <c r="D1278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1279" spans="1:4">
@@ -22383,7 +22383,7 @@
         <v>0</v>
       </c>
       <c r="D1316">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1317" spans="1:4">
@@ -23461,7 +23461,7 @@
         <v>0</v>
       </c>
       <c r="D1393">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1394" spans="1:4">
@@ -23825,7 +23825,7 @@
         <v>1</v>
       </c>
       <c r="D1419">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1420" spans="1:4">
@@ -24049,7 +24049,7 @@
         <v>1</v>
       </c>
       <c r="D1435">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1436" spans="1:4">
@@ -24861,7 +24861,7 @@
         <v>0</v>
       </c>
       <c r="D1493">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1494" spans="1:4">
@@ -25715,7 +25715,7 @@
         <v>1</v>
       </c>
       <c r="D1554">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1555" spans="1:4">
@@ -27353,7 +27353,7 @@
         <v>1</v>
       </c>
       <c r="D1671">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1672" spans="1:4">
@@ -27801,7 +27801,7 @@
         <v>1</v>
       </c>
       <c r="D1703">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1704" spans="1:4">
@@ -27857,7 +27857,7 @@
         <v>1</v>
       </c>
       <c r="D1707">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1708" spans="1:4">
@@ -27955,7 +27955,7 @@
         <v>0</v>
       </c>
       <c r="D1714">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1715" spans="1:4">
@@ -28123,7 +28123,7 @@
         <v>0</v>
       </c>
       <c r="D1726">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1727" spans="1:4">
@@ -28249,7 +28249,7 @@
         <v>0</v>
       </c>
       <c r="D1735">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1736" spans="1:4">
@@ -28263,7 +28263,7 @@
         <v>0</v>
       </c>
       <c r="D1736">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1737" spans="1:4">
@@ -28431,7 +28431,7 @@
         <v>0</v>
       </c>
       <c r="D1748">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1749" spans="1:4">
@@ -28445,7 +28445,7 @@
         <v>0</v>
       </c>
       <c r="D1749">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1750" spans="1:4">
@@ -28739,7 +28739,7 @@
         <v>0</v>
       </c>
       <c r="D1770">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1771" spans="1:4">
@@ -28767,7 +28767,7 @@
         <v>0</v>
       </c>
       <c r="D1772">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1773" spans="1:4">
@@ -28991,7 +28991,7 @@
         <v>0</v>
       </c>
       <c r="D1788">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1789" spans="1:4">
@@ -29005,7 +29005,7 @@
         <v>0</v>
       </c>
       <c r="D1789">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1790" spans="1:4">
@@ -29145,7 +29145,7 @@
         <v>0</v>
       </c>
       <c r="D1799">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1800" spans="1:4">
@@ -29215,7 +29215,7 @@
         <v>0</v>
       </c>
       <c r="D1804">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1805" spans="1:4">
@@ -29341,7 +29341,7 @@
         <v>0</v>
       </c>
       <c r="D1813">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1814" spans="1:4">
@@ -29649,7 +29649,7 @@
         <v>0</v>
       </c>
       <c r="D1835">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1836" spans="1:4">
@@ -29705,7 +29705,7 @@
         <v>0</v>
       </c>
       <c r="D1839">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1840" spans="1:4">
@@ -29845,7 +29845,7 @@
         <v>0</v>
       </c>
       <c r="D1849">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1850" spans="1:4">
@@ -29971,7 +29971,7 @@
         <v>0</v>
       </c>
       <c r="D1858">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1859" spans="1:4">
@@ -30027,7 +30027,7 @@
         <v>1</v>
       </c>
       <c r="D1862">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1863" spans="1:4">
@@ -30041,7 +30041,7 @@
         <v>0</v>
       </c>
       <c r="D1863">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1864" spans="1:4">
@@ -30097,7 +30097,7 @@
         <v>0</v>
       </c>
       <c r="D1867">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1868" spans="1:4">
@@ -30195,7 +30195,7 @@
         <v>0</v>
       </c>
       <c r="D1874">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1875" spans="1:4">
@@ -30279,7 +30279,7 @@
         <v>0</v>
       </c>
       <c r="D1880">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1881" spans="1:4">
@@ -30503,7 +30503,7 @@
         <v>0</v>
       </c>
       <c r="D1896">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1897" spans="1:4">
@@ -30559,7 +30559,7 @@
         <v>0</v>
       </c>
       <c r="D1900">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1901" spans="1:4">
@@ -30811,7 +30811,7 @@
         <v>0</v>
       </c>
       <c r="D1918">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1919" spans="1:4">
@@ -30867,7 +30867,7 @@
         <v>1</v>
       </c>
       <c r="D1922">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1923" spans="1:4">
@@ -31679,7 +31679,7 @@
         <v>1</v>
       </c>
       <c r="D1980">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1981" spans="1:4">
@@ -31693,7 +31693,7 @@
         <v>1</v>
       </c>
       <c r="D1981">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1982" spans="1:4">
@@ -31987,7 +31987,7 @@
         <v>0</v>
       </c>
       <c r="D2002">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2003" spans="1:4">
@@ -32071,7 +32071,7 @@
         <v>0</v>
       </c>
       <c r="D2008">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2009" spans="1:4">
@@ -32393,7 +32393,7 @@
         <v>0</v>
       </c>
       <c r="D2031">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2032" spans="1:4">
@@ -32407,7 +32407,7 @@
         <v>0</v>
       </c>
       <c r="D2032">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2033" spans="1:4">
@@ -32715,7 +32715,7 @@
         <v>0</v>
       </c>
       <c r="D2054">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2055" spans="1:4">
@@ -32911,7 +32911,7 @@
         <v>0</v>
       </c>
       <c r="D2068">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2069" spans="1:4">
@@ -41857,7 +41857,7 @@
         <v>0</v>
       </c>
       <c r="D2707">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2708" spans="1:4">

</xml_diff>